<commit_message>
feature/MS-Webstore: Reformat and clean code
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/UserDetails.xlsx
+++ b/src/test/resources/Data/UserDetails.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Sharma</t>
   </si>
   <si>
-    <t xml:space="preserve">jdsandkjdeagca@gmail.com</t>
+    <t xml:space="preserve">zbvmjdsandkjdeagca@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Anu@123</t>
@@ -85,7 +85,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -115,6 +115,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,7 +178,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -191,7 +198,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -279,7 +286,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -294,7 +301,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -309,7 +316,7 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -326,7 +333,7 @@
       <c r="D2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -352,13 +359,13 @@
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -373,16 +380,17 @@
       <c r="I3" s="5" t="n">
         <v>7293586349</v>
       </c>
-      <c r="J3" s="6" t="b">
+      <c r="J3" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="andkjdeagca@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="bvmjdsandkjdeagca@gmail.com"/>
     <hyperlink ref="D2" r:id="rId2" display="Anu@123"/>
     <hyperlink ref="H2" r:id="rId3" display="11023"/>
-    <hyperlink ref="C3" r:id="rId4" display="andkjdeagca@gmail.com"/>
+    <hyperlink ref="C3" r:id="rId4" display="bvmjdsandkjdeagca@gmail.com"/>
     <hyperlink ref="D3" r:id="rId5" display="Anu@123"/>
     <hyperlink ref="H3" r:id="rId6" display="11023"/>
   </hyperlinks>

</xml_diff>